<commit_message>
Detect Reservation name, and details
</commit_message>
<xml_diff>
--- a/Final Project/Appointment_Reply.xlsx
+++ b/Final Project/Appointment_Reply.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chathuranga/Desktop/Masters Lecture Docs/Text Mining 732A92 /Labs/Text Mining Labs/Final Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B6119A-E144-D64A-A5BA-84D54F926152}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B43C1D-562B-0249-BA9E-8D2E8F8BA1F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3020" yWindow="500" windowWidth="25040" windowHeight="13800" xr2:uid="{5341645D-5F16-424C-A334-9099AC57F5B1}"/>
+    <workbookView xWindow="1620" yWindow="1220" windowWidth="25040" windowHeight="13800" xr2:uid="{5341645D-5F16-424C-A334-9099AC57F5B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Chat</t>
   </si>
@@ -57,18 +57,12 @@
     <t>I'm making the reservation for USER. Okay ? :)</t>
   </si>
   <si>
-    <t>NAME_CHECK</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
     <t>Ohh sorry! So this appointment for USER? Isn't it ?</t>
   </si>
   <si>
-    <t>So could you please tell me person name for the appointment?</t>
-  </si>
-  <si>
     <t>First I need the person name for the appointment :)</t>
   </si>
   <si>
@@ -79,6 +73,27 @@
   </si>
   <si>
     <t xml:space="preserve">Is this appointment for you USER? </t>
+  </si>
+  <si>
+    <t>NAME_CHECK_P</t>
+  </si>
+  <si>
+    <t>NAME_CHECK_NA</t>
+  </si>
+  <si>
+    <t>NAME_CHECK_N</t>
+  </si>
+  <si>
+    <t>Sorry I'm unable find an appointment person name. Could you please tell me the name ?</t>
+  </si>
+  <si>
+    <t>NAME_CHECK_ERROR</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>So could you please tell me the person name for the appointment?</t>
   </si>
 </sst>
 </file>
@@ -433,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC818079-CDB9-FD4D-8F0F-6186B28DA979}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -459,10 +474,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -473,7 +488,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -481,10 +496,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
@@ -495,7 +510,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
@@ -503,10 +518,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
@@ -514,10 +529,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -525,24 +540,35 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed Make Reservation part
</commit_message>
<xml_diff>
--- a/Final Project/Appointment_Reply.xlsx
+++ b/Final Project/Appointment_Reply.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chathuranga/Desktop/Masters Lecture Docs/Text Mining 732A92 /Labs/Text Mining Labs/Final Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B43C1D-562B-0249-BA9E-8D2E8F8BA1F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B8CC22-4C53-9643-BACB-C6BED701F298}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="1220" windowWidth="25040" windowHeight="13800" xr2:uid="{5341645D-5F16-424C-A334-9099AC57F5B1}"/>
+    <workbookView xWindow="7640" yWindow="1380" windowWidth="25040" windowHeight="13800" xr2:uid="{5341645D-5F16-424C-A334-9099AC57F5B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -451,7 +451,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added change and remove reservation
</commit_message>
<xml_diff>
--- a/Final Project/Appointment_Reply.xlsx
+++ b/Final Project/Appointment_Reply.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chathuranga/Desktop/Masters Lecture Docs/Text Mining 732A92 /Labs/Text Mining Labs/Final Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B8CC22-4C53-9643-BACB-C6BED701F298}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A791174C-7387-784B-BCCF-154E44220F0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7640" yWindow="1380" windowWidth="25040" windowHeight="13800" xr2:uid="{5341645D-5F16-424C-A334-9099AC57F5B1}"/>
+    <workbookView xWindow="560" yWindow="960" windowWidth="25040" windowHeight="13800" xr2:uid="{5341645D-5F16-424C-A334-9099AC57F5B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="27">
   <si>
     <t>Chat</t>
   </si>
@@ -54,9 +54,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>I'm making the reservation for USER. Okay ? :)</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -94,6 +91,30 @@
   </si>
   <si>
     <t>So could you please tell me the person name for the appointment?</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was this appointment made for you USER? </t>
+  </si>
+  <si>
+    <t>So was this for you USER?</t>
+  </si>
+  <si>
+    <t>So  was the appointment for USER? Isn't it ?</t>
+  </si>
+  <si>
+    <t>I'm making the appointment for USER. Okay ? :)</t>
+  </si>
+  <si>
+    <t>So could you please tell me the person name for the appointment which you have placed?</t>
+  </si>
+  <si>
+    <t>Ohh okay :) So the appointment was made for USER? Right ? :)</t>
+  </si>
+  <si>
+    <t>Ohh sorry! So this appointment was made for USER? Isn't it ?</t>
   </si>
 </sst>
 </file>
@@ -448,20 +469,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC818079-CDB9-FD4D-8F0F-6186B28DA979}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="64.83203125" customWidth="1"/>
     <col min="2" max="2" width="18.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="3" max="4" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,103 +492,357 @@
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="C14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="D24" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="1" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added evaluation feedback mechanism
</commit_message>
<xml_diff>
--- a/Final Project/Appointment_Reply.xlsx
+++ b/Final Project/Appointment_Reply.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chathuranga/Desktop/Masters Lecture Docs/Text Mining 732A92 /Labs/Text Mining Labs/Final Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02AFFF6E-AC2A-984D-A44C-6AE710F20F07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CD8664-D0AE-494E-AB18-E96C2488CDDB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="540" yWindow="940" windowWidth="25040" windowHeight="13800" xr2:uid="{5341645D-5F16-424C-A334-9099AC57F5B1}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>Ohh sorry! So this appointment for USER? Isn't it ?</t>
-  </si>
-  <si>
     <t>First I need the person name for the appointment :)</t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   </si>
   <si>
     <t>So this appointment was made for USER? Isn't it ?</t>
+  </si>
+  <si>
+    <t>So this appointment for USER? Isn't it ?</t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -493,15 +493,15 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -515,7 +515,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -526,10 +526,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
@@ -540,10 +540,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
@@ -554,10 +554,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
@@ -568,10 +568,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -582,13 +582,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D8" s="1">
         <v>5</v>
@@ -596,10 +596,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>6</v>
@@ -610,10 +610,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>6</v>
@@ -624,10 +624,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>2</v>
@@ -638,10 +638,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>2</v>
@@ -652,10 +652,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>2</v>
@@ -666,10 +666,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>5</v>
@@ -680,10 +680,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>5</v>
@@ -694,13 +694,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D16" s="1">
         <v>6</v>
@@ -708,10 +708,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>6</v>
@@ -722,10 +722,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>6</v>
@@ -736,10 +736,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>2</v>
@@ -750,10 +750,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>2</v>
@@ -764,10 +764,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>2</v>
@@ -778,10 +778,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>5</v>
@@ -792,10 +792,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>5</v>
@@ -806,13 +806,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D24" s="1">
         <v>7</v>
@@ -820,10 +820,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>6</v>
@@ -834,10 +834,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>6</v>

</xml_diff>